<commit_message>
Bag of Holding (finally) Allow Hints on Custom Items and their activities Fixed missing refresh on activity hints
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="114_{084C62C8-F41E-42A4-9D9C-CBB9D7022225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{18ECF4FC-168E-4F34-B868-84B0E73D397A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="114_{732F8BC0-29A2-47A8-B8C6-09A15626B300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7AE6A2D2-B91E-4416-9979-4F7F9E7B84D3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9317" uniqueCount="2102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9323" uniqueCount="2110">
   <si>
     <t>name</t>
   </si>
@@ -7201,6 +7201,31 @@
   </si>
   <si>
     <t>You can't use any action with the move trait.</t>
+  </si>
+  <si>
+    <t>The only move actions you can use while you're prone are Crawl and Stand. Standing up ends the prone condition.</t>
+  </si>
+  <si>
+    <t>You can Take Cover while prone to hunker down and gain cover against ranged attacks, even if you don't have an object to get behind, gaining a +4 circumstance bonus to AC against ranged attacks (but you remain flat-footed).</t>
+  </si>
+  <si>
+    <t>Creatures within 10 feet of the candle receive a -4 status penalty to Lie.
+When first entering the affected area, each creature (including you) must succeed at a DC 26 Will save or be unable to tell any deliberate lies while within 10 feet of the lit candle. This lasts for as long as the candle is lit.</t>
+  </si>
+  <si>
+    <t>You don't need to use your hands to Climb. However, the slippers require decent traction for you to walk on a wall, so they provide no benefit when you're moving across greased, icy, or oiled surfaces.</t>
+  </si>
+  <si>
+    <t>You gain the effects of the detect magic arcane innate spell from your Arcane Sense at the start of each of your turns without needing to cast the spell, and you gain a +2 status bonus to Perception checks to Seek undetected and hidden creatures and to your Perception DC against Hide and Sneak.</t>
+  </si>
+  <si>
+    <t>Athletics, Movement</t>
+  </si>
+  <si>
+    <t>You gain a +2 circumstance bonus to any defenses against being Shoved or Tripped.</t>
+  </si>
+  <si>
+    <t>Fortitude, Reflex</t>
   </si>
 </sst>
 </file>
@@ -24827,7 +24852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="534" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:130" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>2009</v>
       </c>
@@ -24841,7 +24866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="535" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:130" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>2011</v>
       </c>
@@ -24855,7 +24880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="536" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:130" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>2013</v>
       </c>
@@ -24869,7 +24894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="537" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:130" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>2015</v>
       </c>
@@ -24883,7 +24908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="538" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:130" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>2017</v>
       </c>
@@ -24897,7 +24922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="539" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:130" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>2019</v>
       </c>
@@ -25017,7 +25042,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="548" spans="1:270" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:270" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>2038</v>
       </c>
@@ -25235,7 +25260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="549" spans="1:270" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:270" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>2057</v>
       </c>
@@ -25462,7 +25487,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="550" spans="1:270" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:270" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>2060</v>
       </c>
@@ -25689,7 +25714,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="551" spans="1:270" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:270" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>2071</v>
       </c>
@@ -25716,10 +25741,10 @@
   <dimension ref="A1:UE288"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BW29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AZ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CA57" sqref="CA57"/>
+      <selection pane="bottomRight" activeCell="BD5" sqref="BD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29037,42 +29062,6 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AG3" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="AS3" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="AT3" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="AU3" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="AV3" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="AW3" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="AX3" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="AZ3" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="BA3" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="BD3" s="2" t="s">
-        <v>462</v>
-      </c>
       <c r="BI3" s="2" t="s">
         <v>481</v>
       </c>
@@ -29723,42 +29712,6 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AG4" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="AT4" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="AU4" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="AV4" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="AW4" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="AX4" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="AZ4" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="BA4" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="BD4" s="2" t="s">
-        <v>463</v>
-      </c>
       <c r="BE4" s="2" t="s">
         <v>285</v>
       </c>
@@ -30442,6 +30395,42 @@
       <c r="AF5" s="9" t="s">
         <v>377</v>
       </c>
+      <c r="AG5" s="9" t="s">
+        <v>2102</v>
+      </c>
+      <c r="AI5" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="AS5" s="9" t="s">
+        <v>2104</v>
+      </c>
+      <c r="AT5" s="9" t="s">
+        <v>2105</v>
+      </c>
+      <c r="AU5" s="9" t="s">
+        <v>2106</v>
+      </c>
+      <c r="AV5" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="AW5" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="AX5" s="9" t="s">
+        <v>2108</v>
+      </c>
+      <c r="AZ5" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="BA5" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="BD5" s="9" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="6" spans="1:551" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -30498,6 +30487,42 @@
       <c r="AF6" s="3" t="s">
         <v>375</v>
       </c>
+      <c r="AG6" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="AM6" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="AS6" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="AT6" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="AU6" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AV6" s="3" t="s">
+        <v>2107</v>
+      </c>
+      <c r="AW6" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="AX6" s="3" t="s">
+        <v>2109</v>
+      </c>
+      <c r="AZ6" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="BA6" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BD6" s="3" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="7" spans="1:551" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -30509,6 +30534,12 @@
       <c r="I7" s="11" t="s">
         <v>295</v>
       </c>
+      <c r="AS7" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="AU7" s="3" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="8" spans="1:551" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -30525,6 +30556,12 @@
       <c r="I9" s="3">
         <v>-2</v>
       </c>
+      <c r="AS9" s="3">
+        <v>-4</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:551" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -30536,6 +30573,12 @@
       <c r="I10" s="11" t="s">
         <v>281</v>
       </c>
+      <c r="AS10" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AU10" s="3" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="11" spans="1:551" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -30550,6 +30593,9 @@
       <c r="Z11" s="10" t="s">
         <v>2100</v>
       </c>
+      <c r="AG11" s="9" t="s">
+        <v>2103</v>
+      </c>
     </row>
     <row r="12" spans="1:551" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -30563,6 +30609,9 @@
       </c>
       <c r="Z12" s="11" t="s">
         <v>422</v>
+      </c>
+      <c r="AG12" s="3" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:551" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>